<commit_message>
bàn giao lương MT cho đạt
</commit_message>
<xml_diff>
--- a/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplatePhieuLuong_GT.xlsx
+++ b/01.VietSoftHRM/VietSoftHRM/bin/Debug/Template/TemplatePhieuLuong_GT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HRM_Last\01.VS_HRM\01.VietSoftHRM\VietSoftHRM\bin\Debug\lib\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01.SourceCode\02.HRM\01.VietSoftHRM\VietSoftHRM\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42FEB51-25A7-4FB4-B805-D75DE8828860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-120" windowWidth="13125" windowHeight="11760"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GIANTIEP" sheetId="1" r:id="rId1"/>
@@ -22,17 +23,30 @@
     <definedName name="PhieuNhanLuong">GIANTIEP!$A$7:$AM$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">PhieuLuong!$A$1:$E$57</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="B38" authorId="0" shapeId="0">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E38" authorId="0" shapeId="0">
+    <comment ref="E38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -465,7 +479,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,###"/>
     <numFmt numFmtId="165" formatCode="#,###.0;\(#,###.0\);\ ;\ "/>
@@ -687,9 +701,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -704,7 +718,7 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -717,20 +731,20 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="37" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -740,41 +754,38 @@
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="37" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="37" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -801,7 +812,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Salary sheets" xfId="1"/>
+    <cellStyle name="Normal_Salary sheets" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -833,7 +844,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1033" name="Line 5"/>
+        <xdr:cNvPr id="1033" name="Line 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -870,7 +887,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="DSNV"/>
@@ -3272,9 +3289,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3312,9 +3329,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3349,7 +3366,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3384,7 +3401,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3557,89 +3574,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="10" ySplit="6" topLeftCell="AF7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight" activeCell="AI12" sqref="AI12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
-    <col min="18" max="20" width="9.7109375" customWidth="1"/>
-    <col min="21" max="21" width="5.7109375" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="8.7109375" customWidth="1"/>
-    <col min="27" max="30" width="9.7109375" customWidth="1"/>
-    <col min="32" max="34" width="9.7109375" customWidth="1"/>
-    <col min="35" max="35" width="12.140625" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="9" width="9.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" customWidth="1"/>
+    <col min="11" max="11" width="5.7265625" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" customWidth="1"/>
+    <col min="13" max="13" width="5.7265625" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" customWidth="1"/>
+    <col min="16" max="16" width="9.7265625" customWidth="1"/>
+    <col min="18" max="20" width="9.7265625" customWidth="1"/>
+    <col min="21" max="21" width="5.7265625" customWidth="1"/>
+    <col min="22" max="22" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.7265625" customWidth="1"/>
+    <col min="27" max="30" width="9.7265625" customWidth="1"/>
+    <col min="32" max="34" width="9.7265625" customWidth="1"/>
+    <col min="35" max="35" width="12.1796875" customWidth="1"/>
+    <col min="36" max="36" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" ht="14" x14ac:dyDescent="0.4">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:39" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" ht="14" x14ac:dyDescent="0.4">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:39" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="50" t="s">
+    <row r="3" spans="1:39" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="50"/>
-      <c r="S3" s="50"/>
-      <c r="T3" s="50"/>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="50"/>
-      <c r="Z3" s="50"/>
-      <c r="AA3" s="50"/>
-      <c r="AB3" s="50"/>
-      <c r="AC3" s="50"/>
-      <c r="AD3" s="50"/>
-      <c r="AE3" s="50"/>
-      <c r="AF3" s="50"/>
-      <c r="AG3" s="50"/>
-      <c r="AH3" s="50"/>
-      <c r="AI3" s="50"/>
-      <c r="AJ3" s="50"/>
-      <c r="AK3" s="50"/>
-      <c r="AL3" s="50"/>
-    </row>
-    <row r="5" spans="1:39" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="49"/>
+    </row>
+    <row r="5" spans="1:39" ht="27" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -3758,7 +3775,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -3877,113 +3894,113 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" ht="23" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="47" t="s">
         <v>90</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="48" t="s">
         <v>108</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="49" t="s">
+      <c r="I7" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="48" t="s">
         <v>93</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="L7" s="49" t="s">
+      <c r="L7" s="48" t="s">
         <v>95</v>
       </c>
       <c r="M7" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="N7" s="49" t="s">
+      <c r="N7" s="48" t="s">
         <v>110</v>
       </c>
       <c r="O7" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="P7" s="49" t="s">
+      <c r="P7" s="48" t="s">
         <v>112</v>
       </c>
       <c r="Q7" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="R7" s="49" t="s">
+      <c r="R7" s="48" t="s">
         <v>98</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="T7" s="49" t="s">
+      <c r="T7" s="48" t="s">
         <v>113</v>
       </c>
       <c r="U7" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="V7" s="49" t="s">
+      <c r="V7" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="W7" s="49" t="s">
+      <c r="W7" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="X7" s="49" t="s">
+      <c r="X7" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="Y7" s="49" t="s">
+      <c r="Y7" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="Z7" s="49" t="s">
+      <c r="Z7" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="AA7" s="49" t="s">
+      <c r="AA7" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="AB7" s="49" t="s">
+      <c r="AB7" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="AC7" s="49" t="s">
+      <c r="AC7" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="AD7" s="49" t="s">
+      <c r="AD7" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="AE7" s="49" t="s">
+      <c r="AE7" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="AF7" s="49" t="s">
+      <c r="AF7" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="AG7" s="49" t="s">
+      <c r="AG7" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="AH7" s="49" t="s">
+      <c r="AH7" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="AI7" s="49" t="s">
+      <c r="AI7" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="AJ7" s="49" t="s">
+      <c r="AJ7" s="48" t="s">
         <v>105</v>
       </c>
       <c r="AK7" s="5" t="s">
@@ -3992,19 +4009,19 @@
       <c r="AL7" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="AM7" s="49" t="s">
+      <c r="AM7" s="48" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A8" s="51" t="s">
+    <row r="8" spans="1:39" ht="13" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
       <c r="G8" s="9">
         <f t="shared" ref="G8:S8" si="0">SUM(G7:G7)</f>
         <v>0</v>
@@ -4132,7 +4149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="AI10" s="4">
         <f>+AB8-AH8</f>
         <v>0</v>
@@ -4151,23 +4168,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="62.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="61.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.26953125" customWidth="1"/>
+    <col min="3" max="3" width="3.26953125" customWidth="1"/>
+    <col min="4" max="4" width="62.453125" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12"/>
       <c r="B1" s="13">
         <v>1</v>
@@ -4178,37 +4195,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="str">
+    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.5">
+      <c r="A2" s="51" t="str">
         <f ca="1">"PHIEÁU THANH TOAÙN LÖÔNG THAÙNG"&amp;TEXT(TODAY()-20," MM-YYYY")</f>
-        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 04-2022</v>
-      </c>
-      <c r="B2" s="52"/>
-      <c r="D2" s="54" t="str">
+        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 07-2023</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="D2" s="53" t="str">
         <f ca="1">+A2</f>
-        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 04-2022</v>
-      </c>
-      <c r="E2" s="54"/>
-    </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="str">
+        <v>PHIEÁU THANH TOAÙN LÖÔNG THAÙNG 07-2023</v>
+      </c>
+      <c r="E2" s="53"/>
+    </row>
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.45">
+      <c r="A3" s="52" t="str">
         <f ca="1">"(PAYSLIP FOR THE MONTH OF "&amp;TRIM(RIGHT(A2,7))&amp;")"</f>
-        <v>(PAYSLIP FOR THE MONTH OF 04-2022)</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="D3" s="55" t="str">
+        <v>(PAYSLIP FOR THE MONTH OF 07-2023)</v>
+      </c>
+      <c r="B3" s="52"/>
+      <c r="D3" s="54" t="str">
         <f ca="1">+A3</f>
-        <v>(PAYSLIP FOR THE MONTH OF 04-2022)</v>
-      </c>
-      <c r="E3" s="55"/>
-    </row>
-    <row r="4" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>(PAYSLIP FOR THE MONTH OF 07-2023)</v>
+      </c>
+      <c r="E3" s="54"/>
+    </row>
+    <row r="4" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>36</v>
       </c>
@@ -4225,8 +4242,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="15" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:5" s="15" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="29" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="30" t="e">
@@ -4234,7 +4251,7 @@
         <v>#N/A</v>
       </c>
       <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="29" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="30" t="e">
@@ -4242,8 +4259,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="30" t="e">
@@ -4251,7 +4268,7 @@
         <v>#N/A</v>
       </c>
       <c r="C7" s="31"/>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="29" t="s">
         <v>38</v>
       </c>
       <c r="E7" s="30" t="e">
@@ -4259,619 +4276,619 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="33" t="e">
+      <c r="B8" s="32" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,5,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C8" s="31"/>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="33" t="e">
+      <c r="E8" s="32" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,5,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="34" t="e">
+      <c r="B9" s="33" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,7,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C9" s="31"/>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="34" t="e">
+      <c r="E9" s="33" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,7,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:5" s="15" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="34" t="e">
+      <c r="B10" s="33" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,9,0)</f>
         <v>#N/A</v>
       </c>
       <c r="C10" s="31"/>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="34" t="e">
+      <c r="E10" s="33" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,9,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="15" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
+    <row r="12" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="D12" s="35" t="s">
+      <c r="B12" s="35"/>
+      <c r="D12" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="38" t="e">
+      <c r="B13" s="37" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,8,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="38" t="e">
+      <c r="E13" s="37" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,8,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="38" t="e">
+      <c r="B14" s="37" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,17,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="38" t="e">
+      <c r="E14" s="37" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,17,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="37"/>
       <c r="D15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="38"/>
-    </row>
-    <row r="16" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="37"/>
+    </row>
+    <row r="16" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="37"/>
       <c r="D16" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="38"/>
-    </row>
-    <row r="17" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="37"/>
+    </row>
+    <row r="17" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="38" t="e">
+      <c r="B17" s="37" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,19,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="38" t="e">
+      <c r="E17" s="37" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,19,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="31" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="39" t="e">
+      <c r="B18" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,10,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="39" t="e">
+      <c r="E18" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,10,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="39"/>
+      <c r="B19" s="38"/>
       <c r="D19" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="39"/>
-    </row>
-    <row r="20" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="38"/>
+    </row>
+    <row r="20" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="39" t="e">
+      <c r="B20" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,18,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="39" t="e">
+      <c r="E20" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,18,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="39"/>
+      <c r="B21" s="38"/>
       <c r="D21" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="38"/>
+    </row>
+    <row r="22" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="39"/>
+      <c r="B22" s="38"/>
       <c r="D22" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="39"/>
-    </row>
-    <row r="23" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="37" t="s">
+      <c r="E22" s="38"/>
+    </row>
+    <row r="23" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="38" t="e">
+      <c r="B23" s="37" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,11,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="38" t="e">
+      <c r="E23" s="37" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,11,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="39" t="e">
+      <c r="B24" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,12,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="39" t="e">
+      <c r="E24" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,12,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+    <row r="25" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="39" t="e">
+      <c r="B25" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,13,0)+VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,15,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="39" t="e">
+      <c r="E25" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,13,0)+VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,15,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+    <row r="26" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="39" t="e">
+      <c r="B26" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,14,0)+VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,16,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="39" t="e">
+      <c r="E26" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,14,0)+VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,16,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="37"/>
       <c r="D27" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="38"/>
-    </row>
-    <row r="28" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="37"/>
+    </row>
+    <row r="28" spans="1:5" s="31" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="39"/>
+      <c r="B28" s="38"/>
       <c r="D28" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="39"/>
-    </row>
-    <row r="29" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="38"/>
+    </row>
+    <row r="29" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="39" t="e">
+      <c r="B29" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,22,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D29" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="39" t="e">
+      <c r="E29" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,22,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="39" t="e">
+      <c r="B30" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,23,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D30" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="39" t="e">
+      <c r="E30" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,23,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="39" t="e">
+      <c r="B31" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,24,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D31" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="39" t="e">
+      <c r="E31" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,24,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="39" t="e">
+      <c r="B32" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,26,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D32" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="39" t="e">
+      <c r="E32" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,26,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="39" t="e">
+      <c r="B33" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,25,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="39" t="e">
+      <c r="E33" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,25,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="39" t="e">
+      <c r="B34" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,27,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D34" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="39" t="e">
+      <c r="E34" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,27,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="39" t="e">
+      <c r="B35" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AM$923,38,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D35" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="39" t="e">
+      <c r="E35" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AM$923,38,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="39" t="e">
+      <c r="B36" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AM$923,39,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D36" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="39" t="e">
+      <c r="E36" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AM$923,39,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="40" t="s">
+    <row r="37" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="41" t="e">
+      <c r="B37" s="40" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,28,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="41" t="e">
+      <c r="E37" s="40" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,28,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="31" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="31" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="28"/>
-      <c r="B38" s="42" t="e">
+      <c r="B38" s="41" t="e">
         <f>IF(+B18+B19+B23+B24+B27+B28+ROUND(SUM(B29:B34),0)=B37-1,"","Sai")</f>
         <v>#N/A</v>
       </c>
       <c r="D38" s="28"/>
-      <c r="E38" s="42" t="e">
+      <c r="E38" s="41" t="e">
         <f>IF(+E18+E19+E23+E24+E27+E28+ROUND(SUM(E29:E34),0)=E37-1,"","Sai")</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="35" t="s">
+    <row r="39" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="D39" s="35" t="s">
+      <c r="B39" s="42"/>
+      <c r="D39" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="43"/>
-    </row>
-    <row r="40" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
+      <c r="E39" s="42"/>
+    </row>
+    <row r="40" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="39"/>
-      <c r="D40" s="37" t="s">
+      <c r="B40" s="38"/>
+      <c r="D40" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="39"/>
-    </row>
-    <row r="41" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="38"/>
+    </row>
+    <row r="41" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="39" t="e">
+      <c r="B41" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,30,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D41" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E41" s="39" t="e">
+      <c r="E41" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,30,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
+    <row r="42" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="39" t="e">
+      <c r="B42" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,29,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D42" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="39" t="e">
+      <c r="E42" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,29,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
+    <row r="43" spans="1:5" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="39" t="e">
+      <c r="B43" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,32,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="39" t="e">
+      <c r="E43" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,32,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="s">
+    <row r="44" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="39" t="e">
+      <c r="B44" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,31,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="39" t="e">
+      <c r="E44" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,31,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
+    <row r="45" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="39" t="e">
+      <c r="B45" s="38" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,33,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="39" t="e">
+      <c r="E45" s="38" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,33,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="44" t="s">
+    <row r="46" spans="1:5" s="31" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="41" t="e">
+      <c r="B46" s="40" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,34,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="41" t="e">
+      <c r="E46" s="40" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,34,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="45" t="str">
+    <row r="47" spans="1:5" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="44" t="str">
         <f>"Ghi chuù (Note): "&amp;IF(ISNA(VLOOKUP(RIGHT(B5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0)),"",VLOOKUP(RIGHT(B5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0))</f>
         <v xml:space="preserve">Ghi chuù (Note): </v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="D47" s="45" t="str">
+      <c r="B47" s="40"/>
+      <c r="D47" s="44" t="str">
         <f>"Ghi chuù (Note): "&amp;IF(ISNA(VLOOKUP(RIGHT(E5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0)),"",VLOOKUP(RIGHT(E5,4),'[1]Ghi chu dieu chinh'!$B$8:$AL$302,33,0))</f>
         <v xml:space="preserve">Ghi chuù (Note): </v>
       </c>
-      <c r="E47" s="41"/>
-    </row>
-    <row r="48" spans="1:5" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="46" t="s">
+      <c r="E47" s="40"/>
+    </row>
+    <row r="48" spans="1:5" s="31" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="47" t="e">
+      <c r="B48" s="46" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,35,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D48" s="46" t="s">
+      <c r="D48" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="E48" s="47" t="e">
+      <c r="E48" s="46" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,35,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="46" t="s">
+    <row r="49" spans="1:5" s="31" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="B49" s="47" t="e">
+      <c r="B49" s="46" t="e">
         <f>VLOOKUP($B$1,GIANTIEP!$A$7:$AK$923,36,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D49" s="46" t="s">
+      <c r="D49" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="47" t="e">
+      <c r="E49" s="46" t="e">
         <f>VLOOKUP($E$1,GIANTIEP!$A$7:$AK$923,36,0)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" s="15" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="21"/>
       <c r="B50" s="20"/>
       <c r="C50" s="16"/>
       <c r="D50" s="21"/>
       <c r="E50" s="20"/>
     </row>
-    <row r="51" spans="1:5" s="15" customFormat="1" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" s="15" customFormat="1" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="19"/>
       <c r="B51" s="22"/>
       <c r="C51" s="16"/>
       <c r="D51" s="19"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="23" t="s">
         <v>67</v>
       </c>
@@ -4882,14 +4899,14 @@
       </c>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:5" s="15" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" s="15" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="23"/>
       <c r="B53" s="24"/>
       <c r="C53" s="16"/>
       <c r="D53" s="23"/>
       <c r="E53" s="24"/>
     </row>
-    <row r="54" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="25" t="s">
         <v>68</v>
       </c>
@@ -4899,7 +4916,7 @@
       </c>
       <c r="E54" s="26"/>
     </row>
-    <row r="55" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="25" t="s">
         <v>69</v>
       </c>
@@ -4909,7 +4926,7 @@
       </c>
       <c r="E55" s="26"/>
     </row>
-    <row r="56" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="25" t="s">
         <v>70</v>
       </c>
@@ -4919,7 +4936,7 @@
       </c>
       <c r="E56" s="26"/>
     </row>
-    <row r="57" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="27" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="25" t="s">
         <v>71</v>
       </c>

</xml_diff>